<commit_message>
updated layout of page
</commit_message>
<xml_diff>
--- a/Layout.xlsx
+++ b/Layout.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1367" yWindow="0" windowWidth="24233" windowHeight="10253" xr2:uid="{BB0BF283-396A-4C87-9AB1-2474840A99E0}"/>
+    <workbookView xWindow="2733" yWindow="0" windowWidth="24233" windowHeight="10253" xr2:uid="{BB0BF283-396A-4C87-9AB1-2474840A99E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -302,20 +302,20 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -639,28 +639,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFB2EFC8-7A8F-437B-AD16-39756393A014}">
-  <dimension ref="I2:AP33"/>
+  <dimension ref="I2:AO33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="AX13" sqref="AX13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="8" width="4.1171875" style="1"/>
     <col min="9" max="9" width="1.76171875" style="1" customWidth="1"/>
-    <col min="10" max="13" width="4.1171875" style="1"/>
-    <col min="14" max="14" width="2.29296875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="4.1171875" style="1"/>
-    <col min="16" max="16" width="1.234375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="9.29296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="35" width="4.1171875" style="1"/>
-    <col min="36" max="36" width="1.234375" style="1" customWidth="1"/>
-    <col min="37" max="16384" width="4.1171875" style="1"/>
+    <col min="10" max="10" width="2.29296875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="4.1171875" style="1"/>
+    <col min="12" max="12" width="1.234375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.29296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="31" width="4.1171875" style="1"/>
+    <col min="32" max="32" width="1.234375" style="1" customWidth="1"/>
+    <col min="33" max="40" width="4.1171875" style="1"/>
+    <col min="41" max="41" width="1.703125" style="1" customWidth="1"/>
+    <col min="42" max="16384" width="4.1171875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="9:42" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="3" spans="9:42" x14ac:dyDescent="0.5">
+    <row r="2" spans="9:41" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="3" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I3" s="3"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -693,10 +694,9 @@
       <c r="AL3" s="4"/>
       <c r="AM3" s="4"/>
       <c r="AN3" s="4"/>
-      <c r="AO3" s="4"/>
-      <c r="AP3" s="5"/>
-    </row>
-    <row r="4" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AO3" s="5"/>
+    </row>
+    <row r="4" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
@@ -729,64 +729,62 @@
       <c r="AL4" s="7"/>
       <c r="AM4" s="7"/>
       <c r="AN4" s="7"/>
-      <c r="AO4" s="7"/>
-      <c r="AP4" s="8"/>
-    </row>
-    <row r="5" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AO4" s="8"/>
+    </row>
+    <row r="5" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I5" s="6"/>
-      <c r="J5" s="22" t="s">
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="21"/>
+      <c r="W5" s="21"/>
+      <c r="X5" s="21"/>
+      <c r="Y5" s="21"/>
+      <c r="Z5" s="21"/>
+      <c r="AA5" s="21"/>
+      <c r="AB5" s="21"/>
+      <c r="AC5" s="21"/>
+      <c r="AD5" s="21"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="7"/>
+      <c r="AH5" s="7"/>
+      <c r="AI5" s="7"/>
+      <c r="AJ5" s="7"/>
+      <c r="AK5" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="U5" s="14"/>
-      <c r="V5" s="14"/>
-      <c r="W5" s="14"/>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="14"/>
-      <c r="Z5" s="14"/>
-      <c r="AA5" s="14"/>
-      <c r="AB5" s="14"/>
-      <c r="AC5" s="14"/>
-      <c r="AD5" s="14"/>
-      <c r="AE5" s="14"/>
-      <c r="AF5" s="14"/>
-      <c r="AG5" s="14"/>
-      <c r="AH5" s="14"/>
-      <c r="AI5" s="7"/>
-      <c r="AJ5" s="7"/>
-      <c r="AK5" s="7"/>
-      <c r="AL5" s="7"/>
-      <c r="AM5" s="7"/>
-      <c r="AN5" s="7"/>
-      <c r="AO5" s="7"/>
-      <c r="AP5" s="8"/>
-    </row>
-    <row r="6" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AL5" s="23"/>
+      <c r="AM5" s="23"/>
+      <c r="AN5" s="24"/>
+      <c r="AO5" s="8"/>
+    </row>
+    <row r="6" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I6" s="6"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7" t="s">
+      <c r="J6" s="7"/>
+      <c r="K6" s="7" t="s">
         <v>1</v>
       </c>
+      <c r="L6" s="7"/>
+      <c r="M6" s="13">
+        <f ca="1">TODAY()</f>
+        <v>43047</v>
+      </c>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
       <c r="P6" s="7"/>
-      <c r="Q6" s="13">
-        <f ca="1">TODAY()</f>
-        <v>43046</v>
-      </c>
+      <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
@@ -806,19 +804,18 @@
       <c r="AH6" s="7"/>
       <c r="AI6" s="7"/>
       <c r="AJ6" s="7"/>
-      <c r="AK6" s="7"/>
+      <c r="AK6" s="14"/>
       <c r="AL6" s="7"/>
       <c r="AM6" s="7"/>
-      <c r="AN6" s="7"/>
-      <c r="AO6" s="7"/>
-      <c r="AP6" s="8"/>
-    </row>
-    <row r="7" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AN6" s="15"/>
+      <c r="AO6" s="8"/>
+    </row>
+    <row r="7" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I7" s="6"/>
-      <c r="J7" s="17"/>
+      <c r="J7" s="7"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
-      <c r="M7" s="18"/>
+      <c r="M7" s="7"/>
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
@@ -842,24 +839,23 @@
       <c r="AH7" s="7"/>
       <c r="AI7" s="7"/>
       <c r="AJ7" s="7"/>
-      <c r="AK7" s="7"/>
+      <c r="AK7" s="14"/>
       <c r="AL7" s="7"/>
       <c r="AM7" s="7"/>
-      <c r="AN7" s="7"/>
-      <c r="AO7" s="7"/>
-      <c r="AP7" s="8"/>
-    </row>
-    <row r="8" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AN7" s="15"/>
+      <c r="AO7" s="8"/>
+    </row>
+    <row r="8" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I8" s="6"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7" t="s">
+      <c r="J8" s="7"/>
+      <c r="K8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="P8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
       <c r="Q8" s="12"/>
       <c r="R8" s="12"/>
       <c r="S8" s="12"/>
@@ -875,24 +871,23 @@
       <c r="AC8" s="12"/>
       <c r="AD8" s="12"/>
       <c r="AE8" s="12"/>
-      <c r="AF8" s="12"/>
-      <c r="AG8" s="12"/>
-      <c r="AH8" s="12"/>
-      <c r="AI8" s="12"/>
+      <c r="AF8" s="7"/>
+      <c r="AG8" s="7"/>
+      <c r="AH8" s="7"/>
+      <c r="AI8" s="7"/>
       <c r="AJ8" s="7"/>
-      <c r="AK8" s="7"/>
+      <c r="AK8" s="14"/>
       <c r="AL8" s="7"/>
       <c r="AM8" s="7"/>
-      <c r="AN8" s="7"/>
-      <c r="AO8" s="7"/>
-      <c r="AP8" s="8"/>
-    </row>
-    <row r="9" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AN8" s="15"/>
+      <c r="AO8" s="8"/>
+    </row>
+    <row r="9" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I9" s="6"/>
-      <c r="J9" s="17"/>
+      <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
-      <c r="M9" s="18"/>
+      <c r="M9" s="7"/>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
@@ -916,20 +911,19 @@
       <c r="AH9" s="7"/>
       <c r="AI9" s="7"/>
       <c r="AJ9" s="7"/>
-      <c r="AK9" s="7"/>
+      <c r="AK9" s="14"/>
       <c r="AL9" s="7"/>
       <c r="AM9" s="7"/>
-      <c r="AN9" s="7"/>
-      <c r="AO9" s="7"/>
-      <c r="AP9" s="8"/>
-    </row>
-    <row r="10" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AN9" s="15"/>
+      <c r="AO9" s="8"/>
+    </row>
+    <row r="10" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I10" s="6"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
       <c r="Q10" s="12"/>
@@ -951,21 +945,20 @@
       <c r="AG10" s="12"/>
       <c r="AH10" s="12"/>
       <c r="AI10" s="12"/>
-      <c r="AJ10" s="12"/>
-      <c r="AK10" s="12"/>
-      <c r="AL10" s="12"/>
-      <c r="AM10" s="12"/>
-      <c r="AN10" s="7"/>
-      <c r="AO10" s="7"/>
-      <c r="AP10" s="8"/>
-    </row>
-    <row r="11" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AJ10" s="7"/>
+      <c r="AK10" s="14"/>
+      <c r="AL10" s="7"/>
+      <c r="AM10" s="7"/>
+      <c r="AN10" s="15"/>
+      <c r="AO10" s="8"/>
+    </row>
+    <row r="11" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I11" s="6"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
       <c r="Q11" s="12"/>
@@ -987,21 +980,20 @@
       <c r="AG11" s="12"/>
       <c r="AH11" s="12"/>
       <c r="AI11" s="12"/>
-      <c r="AJ11" s="12"/>
-      <c r="AK11" s="12"/>
-      <c r="AL11" s="12"/>
-      <c r="AM11" s="12"/>
-      <c r="AN11" s="7"/>
-      <c r="AO11" s="7"/>
-      <c r="AP11" s="8"/>
-    </row>
-    <row r="12" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AJ11" s="7"/>
+      <c r="AK11" s="14"/>
+      <c r="AL11" s="7"/>
+      <c r="AM11" s="7"/>
+      <c r="AN11" s="15"/>
+      <c r="AO11" s="8"/>
+    </row>
+    <row r="12" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I12" s="6"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
       <c r="Q12" s="12"/>
@@ -1023,21 +1015,20 @@
       <c r="AG12" s="12"/>
       <c r="AH12" s="12"/>
       <c r="AI12" s="12"/>
-      <c r="AJ12" s="12"/>
-      <c r="AK12" s="12"/>
-      <c r="AL12" s="12"/>
-      <c r="AM12" s="12"/>
-      <c r="AN12" s="7"/>
-      <c r="AO12" s="7"/>
-      <c r="AP12" s="8"/>
-    </row>
-    <row r="13" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AJ12" s="7"/>
+      <c r="AK12" s="14"/>
+      <c r="AL12" s="7"/>
+      <c r="AM12" s="7"/>
+      <c r="AN12" s="15"/>
+      <c r="AO12" s="8"/>
+    </row>
+    <row r="13" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I13" s="6"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
       <c r="O13" s="12"/>
       <c r="P13" s="12"/>
       <c r="Q13" s="12"/>
@@ -1059,21 +1050,20 @@
       <c r="AG13" s="12"/>
       <c r="AH13" s="12"/>
       <c r="AI13" s="12"/>
-      <c r="AJ13" s="12"/>
-      <c r="AK13" s="12"/>
-      <c r="AL13" s="12"/>
-      <c r="AM13" s="12"/>
-      <c r="AN13" s="7"/>
-      <c r="AO13" s="7"/>
-      <c r="AP13" s="8"/>
-    </row>
-    <row r="14" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AJ13" s="7"/>
+      <c r="AK13" s="16"/>
+      <c r="AL13" s="17"/>
+      <c r="AM13" s="17"/>
+      <c r="AN13" s="18"/>
+      <c r="AO13" s="8"/>
+    </row>
+    <row r="14" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I14" s="6"/>
       <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="12"/>
@@ -1095,23 +1085,20 @@
       <c r="AG14" s="12"/>
       <c r="AH14" s="12"/>
       <c r="AI14" s="12"/>
-      <c r="AJ14" s="12"/>
-      <c r="AK14" s="12"/>
-      <c r="AL14" s="12"/>
-      <c r="AM14" s="12"/>
+      <c r="AJ14" s="7"/>
+      <c r="AK14" s="7"/>
+      <c r="AL14" s="7"/>
+      <c r="AM14" s="7"/>
       <c r="AN14" s="7"/>
-      <c r="AO14" s="7"/>
-      <c r="AP14" s="8"/>
-    </row>
-    <row r="15" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AO14" s="8"/>
+    </row>
+    <row r="15" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I15" s="6"/>
-      <c r="J15" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
       <c r="Q15" s="12"/>
@@ -1133,21 +1120,22 @@
       <c r="AG15" s="12"/>
       <c r="AH15" s="12"/>
       <c r="AI15" s="12"/>
-      <c r="AJ15" s="12"/>
-      <c r="AK15" s="12"/>
-      <c r="AL15" s="12"/>
-      <c r="AM15" s="12"/>
-      <c r="AN15" s="7"/>
-      <c r="AO15" s="7"/>
-      <c r="AP15" s="8"/>
-    </row>
-    <row r="16" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AJ15" s="7"/>
+      <c r="AK15" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL15" s="23"/>
+      <c r="AM15" s="23"/>
+      <c r="AN15" s="24"/>
+      <c r="AO15" s="8"/>
+    </row>
+    <row r="16" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I16" s="6"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
       <c r="Q16" s="12"/>
@@ -1169,21 +1157,20 @@
       <c r="AG16" s="12"/>
       <c r="AH16" s="12"/>
       <c r="AI16" s="12"/>
-      <c r="AJ16" s="12"/>
-      <c r="AK16" s="12"/>
-      <c r="AL16" s="12"/>
-      <c r="AM16" s="12"/>
-      <c r="AN16" s="7"/>
-      <c r="AO16" s="7"/>
-      <c r="AP16" s="8"/>
-    </row>
-    <row r="17" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AJ16" s="7"/>
+      <c r="AK16" s="14"/>
+      <c r="AL16" s="7"/>
+      <c r="AM16" s="7"/>
+      <c r="AN16" s="15"/>
+      <c r="AO16" s="8"/>
+    </row>
+    <row r="17" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I17" s="6"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="18"/>
-      <c r="N17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
       <c r="Q17" s="12"/>
@@ -1205,21 +1192,20 @@
       <c r="AG17" s="12"/>
       <c r="AH17" s="12"/>
       <c r="AI17" s="12"/>
-      <c r="AJ17" s="12"/>
-      <c r="AK17" s="12"/>
-      <c r="AL17" s="12"/>
-      <c r="AM17" s="12"/>
-      <c r="AN17" s="7"/>
-      <c r="AO17" s="7"/>
-      <c r="AP17" s="8"/>
-    </row>
-    <row r="18" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AJ17" s="7"/>
+      <c r="AK17" s="14"/>
+      <c r="AL17" s="7"/>
+      <c r="AM17" s="7"/>
+      <c r="AN17" s="15"/>
+      <c r="AO17" s="8"/>
+    </row>
+    <row r="18" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I18" s="6"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
       <c r="Q18" s="12"/>
@@ -1241,21 +1227,20 @@
       <c r="AG18" s="12"/>
       <c r="AH18" s="12"/>
       <c r="AI18" s="12"/>
-      <c r="AJ18" s="12"/>
-      <c r="AK18" s="12"/>
-      <c r="AL18" s="12"/>
-      <c r="AM18" s="12"/>
-      <c r="AN18" s="7"/>
-      <c r="AO18" s="7"/>
-      <c r="AP18" s="8"/>
-    </row>
-    <row r="19" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AJ18" s="7"/>
+      <c r="AK18" s="14"/>
+      <c r="AL18" s="7"/>
+      <c r="AM18" s="7"/>
+      <c r="AN18" s="15"/>
+      <c r="AO18" s="8"/>
+    </row>
+    <row r="19" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I19" s="6"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="18"/>
-      <c r="N19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
       <c r="O19" s="12"/>
       <c r="P19" s="12"/>
       <c r="Q19" s="12"/>
@@ -1277,21 +1262,20 @@
       <c r="AG19" s="12"/>
       <c r="AH19" s="12"/>
       <c r="AI19" s="12"/>
-      <c r="AJ19" s="12"/>
-      <c r="AK19" s="12"/>
-      <c r="AL19" s="12"/>
-      <c r="AM19" s="12"/>
-      <c r="AN19" s="7"/>
-      <c r="AO19" s="7"/>
-      <c r="AP19" s="8"/>
-    </row>
-    <row r="20" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AJ19" s="7"/>
+      <c r="AK19" s="14"/>
+      <c r="AL19" s="7"/>
+      <c r="AM19" s="7"/>
+      <c r="AN19" s="15"/>
+      <c r="AO19" s="8"/>
+    </row>
+    <row r="20" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I20" s="6"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="18"/>
-      <c r="N20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
       <c r="Q20" s="12"/>
@@ -1313,21 +1297,20 @@
       <c r="AG20" s="12"/>
       <c r="AH20" s="12"/>
       <c r="AI20" s="12"/>
-      <c r="AJ20" s="12"/>
-      <c r="AK20" s="12"/>
-      <c r="AL20" s="12"/>
-      <c r="AM20" s="12"/>
-      <c r="AN20" s="7"/>
-      <c r="AO20" s="7"/>
-      <c r="AP20" s="8"/>
-    </row>
-    <row r="21" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AJ20" s="7"/>
+      <c r="AK20" s="14"/>
+      <c r="AL20" s="7"/>
+      <c r="AM20" s="7"/>
+      <c r="AN20" s="15"/>
+      <c r="AO20" s="8"/>
+    </row>
+    <row r="21" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I21" s="6"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
       <c r="O21" s="12"/>
       <c r="P21" s="12"/>
       <c r="Q21" s="12"/>
@@ -1349,21 +1332,20 @@
       <c r="AG21" s="12"/>
       <c r="AH21" s="12"/>
       <c r="AI21" s="12"/>
-      <c r="AJ21" s="12"/>
-      <c r="AK21" s="12"/>
-      <c r="AL21" s="12"/>
-      <c r="AM21" s="12"/>
-      <c r="AN21" s="7"/>
-      <c r="AO21" s="7"/>
-      <c r="AP21" s="8"/>
-    </row>
-    <row r="22" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AJ21" s="7"/>
+      <c r="AK21" s="14"/>
+      <c r="AL21" s="7"/>
+      <c r="AM21" s="7"/>
+      <c r="AN21" s="15"/>
+      <c r="AO21" s="8"/>
+    </row>
+    <row r="22" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I22" s="6"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
       <c r="O22" s="12"/>
       <c r="P22" s="12"/>
       <c r="Q22" s="12"/>
@@ -1385,21 +1367,20 @@
       <c r="AG22" s="12"/>
       <c r="AH22" s="12"/>
       <c r="AI22" s="12"/>
-      <c r="AJ22" s="12"/>
-      <c r="AK22" s="12"/>
-      <c r="AL22" s="12"/>
-      <c r="AM22" s="12"/>
-      <c r="AN22" s="7"/>
-      <c r="AO22" s="7"/>
-      <c r="AP22" s="8"/>
-    </row>
-    <row r="23" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AJ22" s="7"/>
+      <c r="AK22" s="14"/>
+      <c r="AL22" s="7"/>
+      <c r="AM22" s="7"/>
+      <c r="AN22" s="15"/>
+      <c r="AO22" s="8"/>
+    </row>
+    <row r="23" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I23" s="6"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
       <c r="O23" s="12"/>
       <c r="P23" s="12"/>
       <c r="Q23" s="12"/>
@@ -1421,21 +1402,20 @@
       <c r="AG23" s="12"/>
       <c r="AH23" s="12"/>
       <c r="AI23" s="12"/>
-      <c r="AJ23" s="12"/>
-      <c r="AK23" s="12"/>
-      <c r="AL23" s="12"/>
-      <c r="AM23" s="12"/>
-      <c r="AN23" s="7"/>
-      <c r="AO23" s="7"/>
-      <c r="AP23" s="8"/>
-    </row>
-    <row r="24" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AJ23" s="7"/>
+      <c r="AK23" s="14"/>
+      <c r="AL23" s="7"/>
+      <c r="AM23" s="7"/>
+      <c r="AN23" s="15"/>
+      <c r="AO23" s="8"/>
+    </row>
+    <row r="24" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I24" s="6"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
       <c r="Q24" s="12"/>
@@ -1457,21 +1437,20 @@
       <c r="AG24" s="12"/>
       <c r="AH24" s="12"/>
       <c r="AI24" s="12"/>
-      <c r="AJ24" s="12"/>
-      <c r="AK24" s="12"/>
-      <c r="AL24" s="12"/>
-      <c r="AM24" s="12"/>
-      <c r="AN24" s="7"/>
-      <c r="AO24" s="7"/>
-      <c r="AP24" s="8"/>
-    </row>
-    <row r="25" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AJ24" s="7"/>
+      <c r="AK24" s="14"/>
+      <c r="AL24" s="7"/>
+      <c r="AM24" s="7"/>
+      <c r="AN24" s="15"/>
+      <c r="AO24" s="8"/>
+    </row>
+    <row r="25" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I25" s="6"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="18"/>
-      <c r="N25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
       <c r="O25" s="12"/>
       <c r="P25" s="12"/>
       <c r="Q25" s="12"/>
@@ -1493,21 +1472,20 @@
       <c r="AG25" s="12"/>
       <c r="AH25" s="12"/>
       <c r="AI25" s="12"/>
-      <c r="AJ25" s="12"/>
-      <c r="AK25" s="12"/>
-      <c r="AL25" s="12"/>
-      <c r="AM25" s="12"/>
-      <c r="AN25" s="7"/>
-      <c r="AO25" s="7"/>
-      <c r="AP25" s="8"/>
-    </row>
-    <row r="26" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AJ25" s="7"/>
+      <c r="AK25" s="14"/>
+      <c r="AL25" s="7"/>
+      <c r="AM25" s="7"/>
+      <c r="AN25" s="15"/>
+      <c r="AO25" s="8"/>
+    </row>
+    <row r="26" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I26" s="6"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
       <c r="O26" s="12"/>
       <c r="P26" s="12"/>
       <c r="Q26" s="12"/>
@@ -1529,21 +1507,20 @@
       <c r="AG26" s="12"/>
       <c r="AH26" s="12"/>
       <c r="AI26" s="12"/>
-      <c r="AJ26" s="12"/>
-      <c r="AK26" s="12"/>
-      <c r="AL26" s="12"/>
-      <c r="AM26" s="12"/>
-      <c r="AN26" s="7"/>
-      <c r="AO26" s="7"/>
-      <c r="AP26" s="8"/>
-    </row>
-    <row r="27" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AJ26" s="7"/>
+      <c r="AK26" s="14"/>
+      <c r="AL26" s="7"/>
+      <c r="AM26" s="7"/>
+      <c r="AN26" s="15"/>
+      <c r="AO26" s="8"/>
+    </row>
+    <row r="27" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I27" s="6"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="21"/>
-      <c r="N27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
       <c r="O27" s="12"/>
       <c r="P27" s="12"/>
       <c r="Q27" s="12"/>
@@ -1565,15 +1542,14 @@
       <c r="AG27" s="12"/>
       <c r="AH27" s="12"/>
       <c r="AI27" s="12"/>
-      <c r="AJ27" s="12"/>
-      <c r="AK27" s="12"/>
-      <c r="AL27" s="12"/>
-      <c r="AM27" s="12"/>
-      <c r="AN27" s="7"/>
-      <c r="AO27" s="7"/>
-      <c r="AP27" s="8"/>
-    </row>
-    <row r="28" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AJ27" s="7"/>
+      <c r="AK27" s="16"/>
+      <c r="AL27" s="17"/>
+      <c r="AM27" s="17"/>
+      <c r="AN27" s="18"/>
+      <c r="AO27" s="8"/>
+    </row>
+    <row r="28" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I28" s="6"/>
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
@@ -1606,17 +1582,14 @@
       <c r="AL28" s="7"/>
       <c r="AM28" s="7"/>
       <c r="AN28" s="7"/>
-      <c r="AO28" s="7"/>
-      <c r="AP28" s="8"/>
-    </row>
-    <row r="29" spans="9:42" ht="28" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="AO28" s="8"/>
+    </row>
+    <row r="29" spans="9:41" ht="28" customHeight="1" x14ac:dyDescent="0.5">
       <c r="I29" s="6"/>
-      <c r="J29" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
       <c r="N29" s="7"/>
       <c r="O29" s="7"/>
       <c r="P29" s="7"/>
@@ -1632,26 +1605,27 @@
       <c r="Z29" s="7"/>
       <c r="AA29" s="7"/>
       <c r="AB29" s="7"/>
-      <c r="AC29" s="7"/>
-      <c r="AD29" s="7"/>
-      <c r="AE29" s="7"/>
-      <c r="AF29" s="7"/>
-      <c r="AG29" s="16" t="s">
+      <c r="AC29" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="AH29" s="16"/>
-      <c r="AI29" s="16"/>
-      <c r="AJ29" s="2"/>
-      <c r="AK29" s="15" t="s">
+      <c r="AD29" s="19"/>
+      <c r="AE29" s="19"/>
+      <c r="AF29" s="2"/>
+      <c r="AG29" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="AL29" s="15"/>
-      <c r="AM29" s="15"/>
-      <c r="AN29" s="7"/>
-      <c r="AO29" s="7"/>
-      <c r="AP29" s="8"/>
-    </row>
-    <row r="30" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AH29" s="20"/>
+      <c r="AI29" s="20"/>
+      <c r="AJ29" s="7"/>
+      <c r="AK29" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="AL29" s="21"/>
+      <c r="AM29" s="21"/>
+      <c r="AN29" s="21"/>
+      <c r="AO29" s="8"/>
+    </row>
+    <row r="30" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I30" s="6"/>
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
@@ -1684,10 +1658,9 @@
       <c r="AL30" s="7"/>
       <c r="AM30" s="7"/>
       <c r="AN30" s="7"/>
-      <c r="AO30" s="7"/>
-      <c r="AP30" s="8"/>
-    </row>
-    <row r="31" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AO30" s="8"/>
+    </row>
+    <row r="31" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I31" s="6"/>
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
@@ -1720,10 +1693,9 @@
       <c r="AL31" s="7"/>
       <c r="AM31" s="7"/>
       <c r="AN31" s="7"/>
-      <c r="AO31" s="7"/>
-      <c r="AP31" s="8"/>
-    </row>
-    <row r="32" spans="9:42" x14ac:dyDescent="0.5">
+      <c r="AO31" s="8"/>
+    </row>
+    <row r="32" spans="9:41" x14ac:dyDescent="0.5">
       <c r="I32" s="6"/>
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
@@ -1756,10 +1728,9 @@
       <c r="AL32" s="7"/>
       <c r="AM32" s="7"/>
       <c r="AN32" s="7"/>
-      <c r="AO32" s="7"/>
-      <c r="AP32" s="8"/>
-    </row>
-    <row r="33" spans="9:42" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="AO32" s="8"/>
+    </row>
+    <row r="33" spans="9:41" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="I33" s="9"/>
       <c r="J33" s="10"/>
       <c r="K33" s="10"/>
@@ -1792,17 +1763,16 @@
       <c r="AL33" s="10"/>
       <c r="AM33" s="10"/>
       <c r="AN33" s="10"/>
-      <c r="AO33" s="10"/>
-      <c r="AP33" s="11"/>
+      <c r="AO33" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="AC29:AE29"/>
     <mergeCell ref="AG29:AI29"/>
-    <mergeCell ref="AK29:AM29"/>
-    <mergeCell ref="T5:AH5"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="J29:M29"/>
+    <mergeCell ref="P5:AD5"/>
+    <mergeCell ref="AK5:AN5"/>
+    <mergeCell ref="AK15:AN15"/>
+    <mergeCell ref="AK29:AN29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>